<commit_message>
Worked on the effects doc. + Cleaned half of the Samurai skills doc.
</commit_message>
<xml_diff>
--- a/GameDesign/Class/_Done/3_Ninja/Documentation/NinjaSkills.xlsx
+++ b/GameDesign/Class/_Done/3_Ninja/Documentation/NinjaSkills.xlsx
@@ -2157,8 +2157,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>